<commit_message>
Header and Flip Sign Dimension and Location KPIs running
</commit_message>
<xml_diff>
--- a/Projects/ALTRIAUS/Data/Fixture_Width_Dimensions_v3.xlsx
+++ b/Projects/ALTRIAUS/Data/Fixture_Width_Dimensions_v3.xlsx
@@ -5,13 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Fixture Width" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Conversion Table" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Header Positions" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="POS smokeless" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Flip Sign Positions" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -55,7 +55,7 @@
     <t xml:space="preserve">Number of Headers</t>
   </si>
   <si>
-    <t xml:space="preserve">Cigarette Positions</t>
+    <t xml:space="preserve">Cigarettes Positions</t>
   </si>
   <si>
     <t xml:space="preserve">Smokeless Positions</t>
@@ -210,9 +210,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -445,10 +445,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7244897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.234693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.6122448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.219387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -524,16 +523,16 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.5051020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.9234693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.3163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.8826530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -614,14 +613,14 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.9795918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added Vapor category KPIs
</commit_message>
<xml_diff>
--- a/Projects/ALTRIAUS/Data/Fixture_Width_Dimensions_v3.xlsx
+++ b/Projects/ALTRIAUS/Data/Fixture_Width_Dimensions_v3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Fixture Width" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">Fixture Width (ft)</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">Smokeless Facings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vapor Facings</t>
   </si>
   <si>
     <t xml:space="preserve">Number of Headers</t>
@@ -210,8 +213,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -456,18 +460,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -480,6 +485,9 @@
       <c r="C1" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -491,6 +499,9 @@
       <c r="C2" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="D2" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -502,6 +513,9 @@
       <c r="C3" s="0" t="n">
         <v>8</v>
       </c>
+      <c r="D3" s="0" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -513,6 +527,9 @@
       <c r="C4" s="0" t="n">
         <v>12</v>
       </c>
+      <c r="D4" s="0" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -522,6 +539,9 @@
         <v>19</v>
       </c>
       <c r="C5" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D5" s="0" t="n">
         <v>16</v>
       </c>
     </row>
@@ -543,27 +563,27 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.9387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -571,10 +591,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -582,10 +602,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -593,10 +613,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -604,7 +624,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -612,7 +632,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -639,15 +659,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -655,7 +676,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -663,7 +684,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>